<commit_message>
corrige excluir tarefa , adiciona modal de excluir projeto e input de filtro de projetos
</commit_message>
<xml_diff>
--- a/backup_projetos.xlsx
+++ b/backup_projetos.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G379"/>
+  <dimension ref="A1:G409"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3247,9 +3247,21 @@
           <t>01/09/2023 às 00:57</t>
         </is>
       </c>
-      <c r="E106" t="inlineStr"/>
-      <c r="F106" t="inlineStr"/>
-      <c r="G106" t="inlineStr"/>
+      <c r="E106" t="inlineStr">
+        <is>
+          <t>https://www.mapacultural.pe.gov.br/agente/50140/</t>
+        </is>
+      </c>
+      <c r="F106" t="inlineStr">
+        <is>
+          <t>https://www.mapacultural.pe.gov.br/files/agent/50140/file/1149831/blob.-0a54fc10d15569ea9a82a41230fab9bb.png</t>
+        </is>
+      </c>
+      <c r="G106" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Maenuel Severino dos Santos </t>
+        </is>
+      </c>
     </row>
     <row r="107">
       <c r="A107" t="inlineStr">
@@ -3272,9 +3284,21 @@
           <t>01/09/2023 às 00:57</t>
         </is>
       </c>
-      <c r="E107" t="inlineStr"/>
-      <c r="F107" t="inlineStr"/>
-      <c r="G107" t="inlineStr"/>
+      <c r="E107" t="inlineStr">
+        <is>
+          <t>https://www.mapacultural.pe.gov.br/agente/50140/</t>
+        </is>
+      </c>
+      <c r="F107" t="inlineStr">
+        <is>
+          <t>https://www.mapacultural.pe.gov.br/files/agent/50140/file/1149831/blob.-0a54fc10d15569ea9a82a41230fab9bb.png</t>
+        </is>
+      </c>
+      <c r="G107" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Maenuel Severino dos Santos </t>
+        </is>
+      </c>
     </row>
     <row r="108">
       <c r="A108" t="inlineStr">
@@ -3297,9 +3321,21 @@
           <t>01/09/2023 às 00:57</t>
         </is>
       </c>
-      <c r="E108" t="inlineStr"/>
-      <c r="F108" t="inlineStr"/>
-      <c r="G108" t="inlineStr"/>
+      <c r="E108" t="inlineStr">
+        <is>
+          <t>https://www.mapacultural.pe.gov.br/agente/50140/</t>
+        </is>
+      </c>
+      <c r="F108" t="inlineStr">
+        <is>
+          <t>https://www.mapacultural.pe.gov.br/files/agent/50140/file/1149831/blob.-0a54fc10d15569ea9a82a41230fab9bb.png</t>
+        </is>
+      </c>
+      <c r="G108" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Maenuel Severino dos Santos </t>
+        </is>
+      </c>
     </row>
     <row r="109">
       <c r="A109" t="inlineStr">
@@ -3322,9 +3358,21 @@
           <t>01/09/2023 às 00:57</t>
         </is>
       </c>
-      <c r="E109" t="inlineStr"/>
-      <c r="F109" t="inlineStr"/>
-      <c r="G109" t="inlineStr"/>
+      <c r="E109" t="inlineStr">
+        <is>
+          <t>https://www.mapacultural.pe.gov.br/agente/50140/</t>
+        </is>
+      </c>
+      <c r="F109" t="inlineStr">
+        <is>
+          <t>https://www.mapacultural.pe.gov.br/files/agent/50140/file/1149831/blob.-0a54fc10d15569ea9a82a41230fab9bb.png</t>
+        </is>
+      </c>
+      <c r="G109" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Maenuel Severino dos Santos </t>
+        </is>
+      </c>
     </row>
     <row r="110">
       <c r="A110" t="inlineStr">
@@ -3339,7 +3387,7 @@
       </c>
       <c r="C110" t="inlineStr">
         <is>
-          <t>Feito</t>
+          <t>Não Feito</t>
         </is>
       </c>
       <c r="D110" t="inlineStr">
@@ -3347,9 +3395,21 @@
           <t>01/09/2023 às 00:57</t>
         </is>
       </c>
-      <c r="E110" t="inlineStr"/>
-      <c r="F110" t="inlineStr"/>
-      <c r="G110" t="inlineStr"/>
+      <c r="E110" t="inlineStr">
+        <is>
+          <t>https://www.mapacultural.pe.gov.br/agente/50140/</t>
+        </is>
+      </c>
+      <c r="F110" t="inlineStr">
+        <is>
+          <t>https://www.mapacultural.pe.gov.br/files/agent/50140/file/1149831/blob.-0a54fc10d15569ea9a82a41230fab9bb.png</t>
+        </is>
+      </c>
+      <c r="G110" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Maenuel Severino dos Santos </t>
+        </is>
+      </c>
     </row>
     <row r="111">
       <c r="A111" t="inlineStr">
@@ -3364,7 +3424,7 @@
       </c>
       <c r="C111" t="inlineStr">
         <is>
-          <t>Feito</t>
+          <t>Não Feito</t>
         </is>
       </c>
       <c r="D111" t="inlineStr">
@@ -3372,9 +3432,21 @@
           <t>01/09/2023 às 00:57</t>
         </is>
       </c>
-      <c r="E111" t="inlineStr"/>
-      <c r="F111" t="inlineStr"/>
-      <c r="G111" t="inlineStr"/>
+      <c r="E111" t="inlineStr">
+        <is>
+          <t>https://www.mapacultural.pe.gov.br/agente/50140/</t>
+        </is>
+      </c>
+      <c r="F111" t="inlineStr">
+        <is>
+          <t>https://www.mapacultural.pe.gov.br/files/agent/50140/file/1149831/blob.-0a54fc10d15569ea9a82a41230fab9bb.png</t>
+        </is>
+      </c>
+      <c r="G111" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Maenuel Severino dos Santos </t>
+        </is>
+      </c>
     </row>
     <row r="112">
       <c r="A112" t="inlineStr">
@@ -3389,7 +3461,7 @@
       </c>
       <c r="C112" t="inlineStr">
         <is>
-          <t>Feito</t>
+          <t>Não Feito</t>
         </is>
       </c>
       <c r="D112" t="inlineStr">
@@ -3397,9 +3469,21 @@
           <t>01/09/2023 às 00:57</t>
         </is>
       </c>
-      <c r="E112" t="inlineStr"/>
-      <c r="F112" t="inlineStr"/>
-      <c r="G112" t="inlineStr"/>
+      <c r="E112" t="inlineStr">
+        <is>
+          <t>https://www.mapacultural.pe.gov.br/agente/50140/</t>
+        </is>
+      </c>
+      <c r="F112" t="inlineStr">
+        <is>
+          <t>https://www.mapacultural.pe.gov.br/files/agent/50140/file/1149831/blob.-0a54fc10d15569ea9a82a41230fab9bb.png</t>
+        </is>
+      </c>
+      <c r="G112" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Maenuel Severino dos Santos </t>
+        </is>
+      </c>
     </row>
     <row r="113">
       <c r="A113" t="inlineStr">
@@ -3414,7 +3498,7 @@
       </c>
       <c r="C113" t="inlineStr">
         <is>
-          <t>Não Feito</t>
+          <t>Feito</t>
         </is>
       </c>
       <c r="D113" t="inlineStr">
@@ -3422,9 +3506,21 @@
           <t>01/09/2023 às 00:57</t>
         </is>
       </c>
-      <c r="E113" t="inlineStr"/>
-      <c r="F113" t="inlineStr"/>
-      <c r="G113" t="inlineStr"/>
+      <c r="E113" t="inlineStr">
+        <is>
+          <t>https://www.mapacultural.pe.gov.br/agente/50140/</t>
+        </is>
+      </c>
+      <c r="F113" t="inlineStr">
+        <is>
+          <t>https://www.mapacultural.pe.gov.br/files/agent/50140/file/1149831/blob.-0a54fc10d15569ea9a82a41230fab9bb.png</t>
+        </is>
+      </c>
+      <c r="G113" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Maenuel Severino dos Santos </t>
+        </is>
+      </c>
     </row>
     <row r="114">
       <c r="A114" t="inlineStr">
@@ -3447,9 +3543,21 @@
           <t>01/09/2023 às 00:57</t>
         </is>
       </c>
-      <c r="E114" t="inlineStr"/>
-      <c r="F114" t="inlineStr"/>
-      <c r="G114" t="inlineStr"/>
+      <c r="E114" t="inlineStr">
+        <is>
+          <t>https://www.mapacultural.pe.gov.br/agente/50140/</t>
+        </is>
+      </c>
+      <c r="F114" t="inlineStr">
+        <is>
+          <t>https://www.mapacultural.pe.gov.br/files/agent/50140/file/1149831/blob.-0a54fc10d15569ea9a82a41230fab9bb.png</t>
+        </is>
+      </c>
+      <c r="G114" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Maenuel Severino dos Santos </t>
+        </is>
+      </c>
     </row>
     <row r="115">
       <c r="A115" t="inlineStr">
@@ -3472,9 +3580,21 @@
           <t>01/09/2023 às 00:57</t>
         </is>
       </c>
-      <c r="E115" t="inlineStr"/>
-      <c r="F115" t="inlineStr"/>
-      <c r="G115" t="inlineStr"/>
+      <c r="E115" t="inlineStr">
+        <is>
+          <t>https://www.mapacultural.pe.gov.br/agente/50140/</t>
+        </is>
+      </c>
+      <c r="F115" t="inlineStr">
+        <is>
+          <t>https://www.mapacultural.pe.gov.br/files/agent/50140/file/1149831/blob.-0a54fc10d15569ea9a82a41230fab9bb.png</t>
+        </is>
+      </c>
+      <c r="G115" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Maenuel Severino dos Santos </t>
+        </is>
+      </c>
     </row>
     <row r="116">
       <c r="A116" t="inlineStr">
@@ -3489,7 +3609,7 @@
       </c>
       <c r="C116" t="inlineStr">
         <is>
-          <t>Não Feito</t>
+          <t>Feito</t>
         </is>
       </c>
       <c r="D116" t="inlineStr">
@@ -3497,9 +3617,21 @@
           <t>01/09/2023 às 00:57</t>
         </is>
       </c>
-      <c r="E116" t="inlineStr"/>
-      <c r="F116" t="inlineStr"/>
-      <c r="G116" t="inlineStr"/>
+      <c r="E116" t="inlineStr">
+        <is>
+          <t>https://www.mapacultural.pe.gov.br/agente/50140/</t>
+        </is>
+      </c>
+      <c r="F116" t="inlineStr">
+        <is>
+          <t>https://www.mapacultural.pe.gov.br/files/agent/50140/file/1149831/blob.-0a54fc10d15569ea9a82a41230fab9bb.png</t>
+        </is>
+      </c>
+      <c r="G116" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Maenuel Severino dos Santos </t>
+        </is>
+      </c>
     </row>
     <row r="117">
       <c r="A117" t="inlineStr">
@@ -3514,7 +3646,7 @@
       </c>
       <c r="C117" t="inlineStr">
         <is>
-          <t>Não Feito</t>
+          <t>Feito</t>
         </is>
       </c>
       <c r="D117" t="inlineStr">
@@ -3522,9 +3654,21 @@
           <t>01/09/2023 às 00:57</t>
         </is>
       </c>
-      <c r="E117" t="inlineStr"/>
-      <c r="F117" t="inlineStr"/>
-      <c r="G117" t="inlineStr"/>
+      <c r="E117" t="inlineStr">
+        <is>
+          <t>https://www.mapacultural.pe.gov.br/agente/50140/</t>
+        </is>
+      </c>
+      <c r="F117" t="inlineStr">
+        <is>
+          <t>https://www.mapacultural.pe.gov.br/files/agent/50140/file/1149831/blob.-0a54fc10d15569ea9a82a41230fab9bb.png</t>
+        </is>
+      </c>
+      <c r="G117" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Maenuel Severino dos Santos </t>
+        </is>
+      </c>
     </row>
     <row r="118">
       <c r="A118" t="inlineStr">
@@ -3547,9 +3691,21 @@
           <t>01/09/2023 às 00:57</t>
         </is>
       </c>
-      <c r="E118" t="inlineStr"/>
-      <c r="F118" t="inlineStr"/>
-      <c r="G118" t="inlineStr"/>
+      <c r="E118" t="inlineStr">
+        <is>
+          <t>https://www.mapacultural.pe.gov.br/agente/50140/</t>
+        </is>
+      </c>
+      <c r="F118" t="inlineStr">
+        <is>
+          <t>https://www.mapacultural.pe.gov.br/files/agent/50140/file/1149831/blob.-0a54fc10d15569ea9a82a41230fab9bb.png</t>
+        </is>
+      </c>
+      <c r="G118" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Maenuel Severino dos Santos </t>
+        </is>
+      </c>
     </row>
     <row r="119">
       <c r="A119" t="inlineStr">
@@ -3572,9 +3728,21 @@
           <t>01/09/2023 às 00:57</t>
         </is>
       </c>
-      <c r="E119" t="inlineStr"/>
-      <c r="F119" t="inlineStr"/>
-      <c r="G119" t="inlineStr"/>
+      <c r="E119" t="inlineStr">
+        <is>
+          <t>https://www.mapacultural.pe.gov.br/agente/38841/</t>
+        </is>
+      </c>
+      <c r="F119" t="inlineStr">
+        <is>
+          <t>https://www.mapacultural.pe.gov.br/files/agent/38841/file/734633/blob-340fa3d2e03e935ef129ffaaaca04b1c.png</t>
+        </is>
+      </c>
+      <c r="G119" t="inlineStr">
+        <is>
+          <t>ELTON LEONARDO DE LIMA GALVÃO</t>
+        </is>
+      </c>
     </row>
     <row r="120">
       <c r="A120" t="inlineStr">
@@ -3597,9 +3765,21 @@
           <t>01/09/2023 às 00:57</t>
         </is>
       </c>
-      <c r="E120" t="inlineStr"/>
-      <c r="F120" t="inlineStr"/>
-      <c r="G120" t="inlineStr"/>
+      <c r="E120" t="inlineStr">
+        <is>
+          <t>https://www.mapacultural.pe.gov.br/agente/38841/</t>
+        </is>
+      </c>
+      <c r="F120" t="inlineStr">
+        <is>
+          <t>https://www.mapacultural.pe.gov.br/files/agent/38841/file/734633/blob-340fa3d2e03e935ef129ffaaaca04b1c.png</t>
+        </is>
+      </c>
+      <c r="G120" t="inlineStr">
+        <is>
+          <t>ELTON LEONARDO DE LIMA GALVÃO</t>
+        </is>
+      </c>
     </row>
     <row r="121">
       <c r="A121" t="inlineStr">
@@ -3614,7 +3794,7 @@
       </c>
       <c r="C121" t="inlineStr">
         <is>
-          <t>Não Feito</t>
+          <t>Feito</t>
         </is>
       </c>
       <c r="D121" t="inlineStr">
@@ -3622,9 +3802,21 @@
           <t>01/09/2023 às 00:57</t>
         </is>
       </c>
-      <c r="E121" t="inlineStr"/>
-      <c r="F121" t="inlineStr"/>
-      <c r="G121" t="inlineStr"/>
+      <c r="E121" t="inlineStr">
+        <is>
+          <t>https://www.mapacultural.pe.gov.br/agente/38841/</t>
+        </is>
+      </c>
+      <c r="F121" t="inlineStr">
+        <is>
+          <t>https://www.mapacultural.pe.gov.br/files/agent/38841/file/734633/blob-340fa3d2e03e935ef129ffaaaca04b1c.png</t>
+        </is>
+      </c>
+      <c r="G121" t="inlineStr">
+        <is>
+          <t>ELTON LEONARDO DE LIMA GALVÃO</t>
+        </is>
+      </c>
     </row>
     <row r="122">
       <c r="A122" t="inlineStr">
@@ -3647,9 +3839,21 @@
           <t>01/09/2023 às 00:57</t>
         </is>
       </c>
-      <c r="E122" t="inlineStr"/>
-      <c r="F122" t="inlineStr"/>
-      <c r="G122" t="inlineStr"/>
+      <c r="E122" t="inlineStr">
+        <is>
+          <t>https://www.mapacultural.pe.gov.br/agente/38841/</t>
+        </is>
+      </c>
+      <c r="F122" t="inlineStr">
+        <is>
+          <t>https://www.mapacultural.pe.gov.br/files/agent/38841/file/734633/blob-340fa3d2e03e935ef129ffaaaca04b1c.png</t>
+        </is>
+      </c>
+      <c r="G122" t="inlineStr">
+        <is>
+          <t>ELTON LEONARDO DE LIMA GALVÃO</t>
+        </is>
+      </c>
     </row>
     <row r="123">
       <c r="A123" t="inlineStr">
@@ -3672,9 +3876,21 @@
           <t>01/09/2023 às 00:57</t>
         </is>
       </c>
-      <c r="E123" t="inlineStr"/>
-      <c r="F123" t="inlineStr"/>
-      <c r="G123" t="inlineStr"/>
+      <c r="E123" t="inlineStr">
+        <is>
+          <t>https://www.mapacultural.pe.gov.br/agente/38841/</t>
+        </is>
+      </c>
+      <c r="F123" t="inlineStr">
+        <is>
+          <t>https://www.mapacultural.pe.gov.br/files/agent/38841/file/734633/blob-340fa3d2e03e935ef129ffaaaca04b1c.png</t>
+        </is>
+      </c>
+      <c r="G123" t="inlineStr">
+        <is>
+          <t>ELTON LEONARDO DE LIMA GALVÃO</t>
+        </is>
+      </c>
     </row>
     <row r="124">
       <c r="A124" t="inlineStr">
@@ -3689,7 +3905,7 @@
       </c>
       <c r="C124" t="inlineStr">
         <is>
-          <t>Não Feito</t>
+          <t>Feito</t>
         </is>
       </c>
       <c r="D124" t="inlineStr">
@@ -3697,9 +3913,21 @@
           <t>01/09/2023 às 00:57</t>
         </is>
       </c>
-      <c r="E124" t="inlineStr"/>
-      <c r="F124" t="inlineStr"/>
-      <c r="G124" t="inlineStr"/>
+      <c r="E124" t="inlineStr">
+        <is>
+          <t>https://www.mapacultural.pe.gov.br/agente/38841/</t>
+        </is>
+      </c>
+      <c r="F124" t="inlineStr">
+        <is>
+          <t>https://www.mapacultural.pe.gov.br/files/agent/38841/file/734633/blob-340fa3d2e03e935ef129ffaaaca04b1c.png</t>
+        </is>
+      </c>
+      <c r="G124" t="inlineStr">
+        <is>
+          <t>ELTON LEONARDO DE LIMA GALVÃO</t>
+        </is>
+      </c>
     </row>
     <row r="125">
       <c r="A125" t="inlineStr">
@@ -3714,7 +3942,7 @@
       </c>
       <c r="C125" t="inlineStr">
         <is>
-          <t>Não Feito</t>
+          <t>Feito</t>
         </is>
       </c>
       <c r="D125" t="inlineStr">
@@ -3722,9 +3950,21 @@
           <t>01/09/2023 às 00:57</t>
         </is>
       </c>
-      <c r="E125" t="inlineStr"/>
-      <c r="F125" t="inlineStr"/>
-      <c r="G125" t="inlineStr"/>
+      <c r="E125" t="inlineStr">
+        <is>
+          <t>https://www.mapacultural.pe.gov.br/agente/38841/</t>
+        </is>
+      </c>
+      <c r="F125" t="inlineStr">
+        <is>
+          <t>https://www.mapacultural.pe.gov.br/files/agent/38841/file/734633/blob-340fa3d2e03e935ef129ffaaaca04b1c.png</t>
+        </is>
+      </c>
+      <c r="G125" t="inlineStr">
+        <is>
+          <t>ELTON LEONARDO DE LIMA GALVÃO</t>
+        </is>
+      </c>
     </row>
     <row r="126">
       <c r="A126" t="inlineStr">
@@ -3747,9 +3987,21 @@
           <t>01/09/2023 às 00:57</t>
         </is>
       </c>
-      <c r="E126" t="inlineStr"/>
-      <c r="F126" t="inlineStr"/>
-      <c r="G126" t="inlineStr"/>
+      <c r="E126" t="inlineStr">
+        <is>
+          <t>https://www.mapacultural.pe.gov.br/agente/38841/</t>
+        </is>
+      </c>
+      <c r="F126" t="inlineStr">
+        <is>
+          <t>https://www.mapacultural.pe.gov.br/files/agent/38841/file/734633/blob-340fa3d2e03e935ef129ffaaaca04b1c.png</t>
+        </is>
+      </c>
+      <c r="G126" t="inlineStr">
+        <is>
+          <t>ELTON LEONARDO DE LIMA GALVÃO</t>
+        </is>
+      </c>
     </row>
     <row r="127">
       <c r="A127" t="inlineStr">
@@ -3764,7 +4016,7 @@
       </c>
       <c r="C127" t="inlineStr">
         <is>
-          <t>Não Feito</t>
+          <t>Feito</t>
         </is>
       </c>
       <c r="D127" t="inlineStr">
@@ -3772,9 +4024,21 @@
           <t>01/09/2023 às 00:57</t>
         </is>
       </c>
-      <c r="E127" t="inlineStr"/>
-      <c r="F127" t="inlineStr"/>
-      <c r="G127" t="inlineStr"/>
+      <c r="E127" t="inlineStr">
+        <is>
+          <t>https://www.mapacultural.pe.gov.br/agente/38841/</t>
+        </is>
+      </c>
+      <c r="F127" t="inlineStr">
+        <is>
+          <t>https://www.mapacultural.pe.gov.br/files/agent/38841/file/734633/blob-340fa3d2e03e935ef129ffaaaca04b1c.png</t>
+        </is>
+      </c>
+      <c r="G127" t="inlineStr">
+        <is>
+          <t>ELTON LEONARDO DE LIMA GALVÃO</t>
+        </is>
+      </c>
     </row>
     <row r="128">
       <c r="A128" t="inlineStr">
@@ -3789,7 +4053,7 @@
       </c>
       <c r="C128" t="inlineStr">
         <is>
-          <t>Não Feito</t>
+          <t>Feito</t>
         </is>
       </c>
       <c r="D128" t="inlineStr">
@@ -3797,9 +4061,21 @@
           <t>01/09/2023 às 00:57</t>
         </is>
       </c>
-      <c r="E128" t="inlineStr"/>
-      <c r="F128" t="inlineStr"/>
-      <c r="G128" t="inlineStr"/>
+      <c r="E128" t="inlineStr">
+        <is>
+          <t>https://www.mapacultural.pe.gov.br/agente/38841/</t>
+        </is>
+      </c>
+      <c r="F128" t="inlineStr">
+        <is>
+          <t>https://www.mapacultural.pe.gov.br/files/agent/38841/file/734633/blob-340fa3d2e03e935ef129ffaaaca04b1c.png</t>
+        </is>
+      </c>
+      <c r="G128" t="inlineStr">
+        <is>
+          <t>ELTON LEONARDO DE LIMA GALVÃO</t>
+        </is>
+      </c>
     </row>
     <row r="129">
       <c r="A129" t="inlineStr">
@@ -3814,7 +4090,7 @@
       </c>
       <c r="C129" t="inlineStr">
         <is>
-          <t>Não Feito</t>
+          <t>Feito</t>
         </is>
       </c>
       <c r="D129" t="inlineStr">
@@ -3822,9 +4098,21 @@
           <t>01/09/2023 às 00:57</t>
         </is>
       </c>
-      <c r="E129" t="inlineStr"/>
-      <c r="F129" t="inlineStr"/>
-      <c r="G129" t="inlineStr"/>
+      <c r="E129" t="inlineStr">
+        <is>
+          <t>https://www.mapacultural.pe.gov.br/agente/38841/</t>
+        </is>
+      </c>
+      <c r="F129" t="inlineStr">
+        <is>
+          <t>https://www.mapacultural.pe.gov.br/files/agent/38841/file/734633/blob-340fa3d2e03e935ef129ffaaaca04b1c.png</t>
+        </is>
+      </c>
+      <c r="G129" t="inlineStr">
+        <is>
+          <t>ELTON LEONARDO DE LIMA GALVÃO</t>
+        </is>
+      </c>
     </row>
     <row r="130">
       <c r="A130" t="inlineStr">
@@ -3839,7 +4127,7 @@
       </c>
       <c r="C130" t="inlineStr">
         <is>
-          <t>Não Feito</t>
+          <t>Feito</t>
         </is>
       </c>
       <c r="D130" t="inlineStr">
@@ -3847,9 +4135,21 @@
           <t>01/09/2023 às 00:57</t>
         </is>
       </c>
-      <c r="E130" t="inlineStr"/>
-      <c r="F130" t="inlineStr"/>
-      <c r="G130" t="inlineStr"/>
+      <c r="E130" t="inlineStr">
+        <is>
+          <t>https://www.mapacultural.pe.gov.br/agente/38841/</t>
+        </is>
+      </c>
+      <c r="F130" t="inlineStr">
+        <is>
+          <t>https://www.mapacultural.pe.gov.br/files/agent/38841/file/734633/blob-340fa3d2e03e935ef129ffaaaca04b1c.png</t>
+        </is>
+      </c>
+      <c r="G130" t="inlineStr">
+        <is>
+          <t>ELTON LEONARDO DE LIMA GALVÃO</t>
+        </is>
+      </c>
     </row>
     <row r="131">
       <c r="A131" t="inlineStr">
@@ -3864,7 +4164,7 @@
       </c>
       <c r="C131" t="inlineStr">
         <is>
-          <t>Não Feito</t>
+          <t>Feito</t>
         </is>
       </c>
       <c r="D131" t="inlineStr">
@@ -3872,9 +4172,21 @@
           <t>01/09/2023 às 00:57</t>
         </is>
       </c>
-      <c r="E131" t="inlineStr"/>
-      <c r="F131" t="inlineStr"/>
-      <c r="G131" t="inlineStr"/>
+      <c r="E131" t="inlineStr">
+        <is>
+          <t>https://www.mapacultural.pe.gov.br/agente/38841/</t>
+        </is>
+      </c>
+      <c r="F131" t="inlineStr">
+        <is>
+          <t>https://www.mapacultural.pe.gov.br/files/agent/38841/file/734633/blob-340fa3d2e03e935ef129ffaaaca04b1c.png</t>
+        </is>
+      </c>
+      <c r="G131" t="inlineStr">
+        <is>
+          <t>ELTON LEONARDO DE LIMA GALVÃO</t>
+        </is>
+      </c>
     </row>
     <row r="132">
       <c r="A132" t="inlineStr">
@@ -10387,6 +10699,1068 @@
       <c r="E379" t="inlineStr"/>
       <c r="F379" t="inlineStr"/>
       <c r="G379" t="inlineStr"/>
+    </row>
+    <row r="380">
+      <c r="A380" t="inlineStr">
+        <is>
+          <t>Artista Elisangela Monteiro</t>
+        </is>
+      </c>
+      <c r="B380" t="inlineStr">
+        <is>
+          <t>RG</t>
+        </is>
+      </c>
+      <c r="C380" t="inlineStr">
+        <is>
+          <t>Não Feito</t>
+        </is>
+      </c>
+      <c r="D380" t="inlineStr">
+        <is>
+          <t>01/09/2023 às 17:55</t>
+        </is>
+      </c>
+      <c r="E380" t="inlineStr">
+        <is>
+          <t>https://www.mapacultural.pe.gov.br/agente/16301/</t>
+        </is>
+      </c>
+      <c r="F380" t="inlineStr">
+        <is>
+          <t>https://www.mapacultural.pe.gov.br/assets/www.mapacultural.pe.gov.br/img/avatar--agent-2487234669-1693235595.png</t>
+        </is>
+      </c>
+      <c r="G380" t="inlineStr">
+        <is>
+          <t>elisangela monteiro de melo costa</t>
+        </is>
+      </c>
+    </row>
+    <row r="381">
+      <c r="A381" t="inlineStr">
+        <is>
+          <t>Artista Elisangela Monteiro</t>
+        </is>
+      </c>
+      <c r="B381" t="inlineStr">
+        <is>
+          <t>CPF</t>
+        </is>
+      </c>
+      <c r="C381" t="inlineStr">
+        <is>
+          <t>Não Feito</t>
+        </is>
+      </c>
+      <c r="D381" t="inlineStr">
+        <is>
+          <t>01/09/2023 às 17:55</t>
+        </is>
+      </c>
+      <c r="E381" t="inlineStr">
+        <is>
+          <t>https://www.mapacultural.pe.gov.br/agente/16301/</t>
+        </is>
+      </c>
+      <c r="F381" t="inlineStr">
+        <is>
+          <t>https://www.mapacultural.pe.gov.br/assets/www.mapacultural.pe.gov.br/img/avatar--agent-2487234669-1693235595.png</t>
+        </is>
+      </c>
+      <c r="G381" t="inlineStr">
+        <is>
+          <t>elisangela monteiro de melo costa</t>
+        </is>
+      </c>
+    </row>
+    <row r="382">
+      <c r="A382" t="inlineStr">
+        <is>
+          <t>Artista Elisangela Monteiro</t>
+        </is>
+      </c>
+      <c r="B382" t="inlineStr">
+        <is>
+          <t>Comprovante de Residência Atual</t>
+        </is>
+      </c>
+      <c r="C382" t="inlineStr">
+        <is>
+          <t>Não Feito</t>
+        </is>
+      </c>
+      <c r="D382" t="inlineStr">
+        <is>
+          <t>01/09/2023 às 17:55</t>
+        </is>
+      </c>
+      <c r="E382" t="inlineStr">
+        <is>
+          <t>https://www.mapacultural.pe.gov.br/agente/16301/</t>
+        </is>
+      </c>
+      <c r="F382" t="inlineStr">
+        <is>
+          <t>https://www.mapacultural.pe.gov.br/assets/www.mapacultural.pe.gov.br/img/avatar--agent-2487234669-1693235595.png</t>
+        </is>
+      </c>
+      <c r="G382" t="inlineStr">
+        <is>
+          <t>elisangela monteiro de melo costa</t>
+        </is>
+      </c>
+    </row>
+    <row r="383">
+      <c r="A383" t="inlineStr">
+        <is>
+          <t>Artista Elisangela Monteiro</t>
+        </is>
+      </c>
+      <c r="B383" t="inlineStr">
+        <is>
+          <t>Comprovações Artísticas</t>
+        </is>
+      </c>
+      <c r="C383" t="inlineStr">
+        <is>
+          <t>Não Feito</t>
+        </is>
+      </c>
+      <c r="D383" t="inlineStr">
+        <is>
+          <t>01/09/2023 às 17:55</t>
+        </is>
+      </c>
+      <c r="E383" t="inlineStr">
+        <is>
+          <t>https://www.mapacultural.pe.gov.br/agente/16301/</t>
+        </is>
+      </c>
+      <c r="F383" t="inlineStr">
+        <is>
+          <t>https://www.mapacultural.pe.gov.br/assets/www.mapacultural.pe.gov.br/img/avatar--agent-2487234669-1693235595.png</t>
+        </is>
+      </c>
+      <c r="G383" t="inlineStr">
+        <is>
+          <t>elisangela monteiro de melo costa</t>
+        </is>
+      </c>
+    </row>
+    <row r="384">
+      <c r="A384" t="inlineStr">
+        <is>
+          <t>Artista Elisangela Monteiro</t>
+        </is>
+      </c>
+      <c r="B384" t="inlineStr">
+        <is>
+          <t>Currículo Artístico</t>
+        </is>
+      </c>
+      <c r="C384" t="inlineStr">
+        <is>
+          <t>Não Feito</t>
+        </is>
+      </c>
+      <c r="D384" t="inlineStr">
+        <is>
+          <t>01/09/2023 às 17:55</t>
+        </is>
+      </c>
+      <c r="E384" t="inlineStr">
+        <is>
+          <t>https://www.mapacultural.pe.gov.br/agente/16301/</t>
+        </is>
+      </c>
+      <c r="F384" t="inlineStr">
+        <is>
+          <t>https://www.mapacultural.pe.gov.br/assets/www.mapacultural.pe.gov.br/img/avatar--agent-2487234669-1693235595.png</t>
+        </is>
+      </c>
+      <c r="G384" t="inlineStr">
+        <is>
+          <t>elisangela monteiro de melo costa</t>
+        </is>
+      </c>
+    </row>
+    <row r="385">
+      <c r="A385" t="inlineStr">
+        <is>
+          <t>Artista Elisangela Monteiro</t>
+        </is>
+      </c>
+      <c r="B385" t="inlineStr">
+        <is>
+          <t>Histórico Atualizado (Ano de Início)</t>
+        </is>
+      </c>
+      <c r="C385" t="inlineStr">
+        <is>
+          <t>Não Feito</t>
+        </is>
+      </c>
+      <c r="D385" t="inlineStr">
+        <is>
+          <t>01/09/2023 às 17:55</t>
+        </is>
+      </c>
+      <c r="E385" t="inlineStr">
+        <is>
+          <t>https://www.mapacultural.pe.gov.br/agente/16301/</t>
+        </is>
+      </c>
+      <c r="F385" t="inlineStr">
+        <is>
+          <t>https://www.mapacultural.pe.gov.br/assets/www.mapacultural.pe.gov.br/img/avatar--agent-2487234669-1693235595.png</t>
+        </is>
+      </c>
+      <c r="G385" t="inlineStr">
+        <is>
+          <t>elisangela monteiro de melo costa</t>
+        </is>
+      </c>
+    </row>
+    <row r="386">
+      <c r="A386" t="inlineStr">
+        <is>
+          <t>Artista Elisangela Monteiro</t>
+        </is>
+      </c>
+      <c r="B386" t="inlineStr">
+        <is>
+          <t>Cadastro Mapa Cultural</t>
+        </is>
+      </c>
+      <c r="C386" t="inlineStr">
+        <is>
+          <t>Feito</t>
+        </is>
+      </c>
+      <c r="D386" t="inlineStr">
+        <is>
+          <t>01/09/2023 às 17:55</t>
+        </is>
+      </c>
+      <c r="E386" t="inlineStr">
+        <is>
+          <t>https://www.mapacultural.pe.gov.br/agente/16301/</t>
+        </is>
+      </c>
+      <c r="F386" t="inlineStr">
+        <is>
+          <t>https://www.mapacultural.pe.gov.br/assets/www.mapacultural.pe.gov.br/img/avatar--agent-2487234669-1693235595.png</t>
+        </is>
+      </c>
+      <c r="G386" t="inlineStr">
+        <is>
+          <t>elisangela monteiro de melo costa</t>
+        </is>
+      </c>
+    </row>
+    <row r="387">
+      <c r="A387" t="inlineStr">
+        <is>
+          <t>Artista Elisangela Monteiro</t>
+        </is>
+      </c>
+      <c r="B387" t="inlineStr">
+        <is>
+          <t>Número Telefone</t>
+        </is>
+      </c>
+      <c r="C387" t="inlineStr">
+        <is>
+          <t>Não Feito</t>
+        </is>
+      </c>
+      <c r="D387" t="inlineStr">
+        <is>
+          <t>01/09/2023 às 17:55</t>
+        </is>
+      </c>
+      <c r="E387" t="inlineStr">
+        <is>
+          <t>https://www.mapacultural.pe.gov.br/agente/16301/</t>
+        </is>
+      </c>
+      <c r="F387" t="inlineStr">
+        <is>
+          <t>https://www.mapacultural.pe.gov.br/assets/www.mapacultural.pe.gov.br/img/avatar--agent-2487234669-1693235595.png</t>
+        </is>
+      </c>
+      <c r="G387" t="inlineStr">
+        <is>
+          <t>elisangela monteiro de melo costa</t>
+        </is>
+      </c>
+    </row>
+    <row r="388">
+      <c r="A388" t="inlineStr">
+        <is>
+          <t>Artista Elisangela Monteiro</t>
+        </is>
+      </c>
+      <c r="B388" t="inlineStr">
+        <is>
+          <t>Cor</t>
+        </is>
+      </c>
+      <c r="C388" t="inlineStr">
+        <is>
+          <t>Não Feito</t>
+        </is>
+      </c>
+      <c r="D388" t="inlineStr">
+        <is>
+          <t>01/09/2023 às 17:55</t>
+        </is>
+      </c>
+      <c r="E388" t="inlineStr">
+        <is>
+          <t>https://www.mapacultural.pe.gov.br/agente/16301/</t>
+        </is>
+      </c>
+      <c r="F388" t="inlineStr">
+        <is>
+          <t>https://www.mapacultural.pe.gov.br/assets/www.mapacultural.pe.gov.br/img/avatar--agent-2487234669-1693235595.png</t>
+        </is>
+      </c>
+      <c r="G388" t="inlineStr">
+        <is>
+          <t>elisangela monteiro de melo costa</t>
+        </is>
+      </c>
+    </row>
+    <row r="389">
+      <c r="A389" t="inlineStr">
+        <is>
+          <t>Artista Elisangela Monteiro</t>
+        </is>
+      </c>
+      <c r="B389" t="inlineStr">
+        <is>
+          <t>Gênero</t>
+        </is>
+      </c>
+      <c r="C389" t="inlineStr">
+        <is>
+          <t>Não Feito</t>
+        </is>
+      </c>
+      <c r="D389" t="inlineStr">
+        <is>
+          <t>01/09/2023 às 17:55</t>
+        </is>
+      </c>
+      <c r="E389" t="inlineStr">
+        <is>
+          <t>https://www.mapacultural.pe.gov.br/agente/16301/</t>
+        </is>
+      </c>
+      <c r="F389" t="inlineStr">
+        <is>
+          <t>https://www.mapacultural.pe.gov.br/assets/www.mapacultural.pe.gov.br/img/avatar--agent-2487234669-1693235595.png</t>
+        </is>
+      </c>
+      <c r="G389" t="inlineStr">
+        <is>
+          <t>elisangela monteiro de melo costa</t>
+        </is>
+      </c>
+    </row>
+    <row r="390">
+      <c r="A390" t="inlineStr">
+        <is>
+          <t>Artista Elisangela Monteiro</t>
+        </is>
+      </c>
+      <c r="B390" t="inlineStr">
+        <is>
+          <t>Grau de Escolaridade</t>
+        </is>
+      </c>
+      <c r="C390" t="inlineStr">
+        <is>
+          <t>Não Feito</t>
+        </is>
+      </c>
+      <c r="D390" t="inlineStr">
+        <is>
+          <t>01/09/2023 às 17:55</t>
+        </is>
+      </c>
+      <c r="E390" t="inlineStr">
+        <is>
+          <t>https://www.mapacultural.pe.gov.br/agente/16301/</t>
+        </is>
+      </c>
+      <c r="F390" t="inlineStr">
+        <is>
+          <t>https://www.mapacultural.pe.gov.br/assets/www.mapacultural.pe.gov.br/img/avatar--agent-2487234669-1693235595.png</t>
+        </is>
+      </c>
+      <c r="G390" t="inlineStr">
+        <is>
+          <t>elisangela monteiro de melo costa</t>
+        </is>
+      </c>
+    </row>
+    <row r="391">
+      <c r="A391" t="inlineStr">
+        <is>
+          <t>Artista Elisangela Monteiro</t>
+        </is>
+      </c>
+      <c r="B391" t="inlineStr">
+        <is>
+          <t>Recebe algum benefício do governo?</t>
+        </is>
+      </c>
+      <c r="C391" t="inlineStr">
+        <is>
+          <t>Não Feito</t>
+        </is>
+      </c>
+      <c r="D391" t="inlineStr">
+        <is>
+          <t>01/09/2023 às 17:55</t>
+        </is>
+      </c>
+      <c r="E391" t="inlineStr">
+        <is>
+          <t>https://www.mapacultural.pe.gov.br/agente/16301/</t>
+        </is>
+      </c>
+      <c r="F391" t="inlineStr">
+        <is>
+          <t>https://www.mapacultural.pe.gov.br/assets/www.mapacultural.pe.gov.br/img/avatar--agent-2487234669-1693235595.png</t>
+        </is>
+      </c>
+      <c r="G391" t="inlineStr">
+        <is>
+          <t>elisangela monteiro de melo costa</t>
+        </is>
+      </c>
+    </row>
+    <row r="392">
+      <c r="A392" t="inlineStr">
+        <is>
+          <t>Artista Elisangela Monteiro</t>
+        </is>
+      </c>
+      <c r="B392" t="inlineStr">
+        <is>
+          <t>Recebeu recursos públicos últimos 5 anos?</t>
+        </is>
+      </c>
+      <c r="C392" t="inlineStr">
+        <is>
+          <t>Não Feito</t>
+        </is>
+      </c>
+      <c r="D392" t="inlineStr">
+        <is>
+          <t>01/09/2023 às 17:55</t>
+        </is>
+      </c>
+      <c r="E392" t="inlineStr">
+        <is>
+          <t>https://www.mapacultural.pe.gov.br/agente/16301/</t>
+        </is>
+      </c>
+      <c r="F392" t="inlineStr">
+        <is>
+          <t>https://www.mapacultural.pe.gov.br/assets/www.mapacultural.pe.gov.br/img/avatar--agent-2487234669-1693235595.png</t>
+        </is>
+      </c>
+      <c r="G392" t="inlineStr">
+        <is>
+          <t>elisangela monteiro de melo costa</t>
+        </is>
+      </c>
+    </row>
+    <row r="393">
+      <c r="A393" t="inlineStr">
+        <is>
+          <t>Artista Marcelo Stallone</t>
+        </is>
+      </c>
+      <c r="B393" t="inlineStr">
+        <is>
+          <t>RG</t>
+        </is>
+      </c>
+      <c r="C393" t="inlineStr">
+        <is>
+          <t>Não Feito</t>
+        </is>
+      </c>
+      <c r="D393" t="inlineStr">
+        <is>
+          <t>01/09/2023 às 17:57</t>
+        </is>
+      </c>
+      <c r="E393" t="inlineStr">
+        <is>
+          <t>https://www.mapacultural.pe.gov.br/agente/39532/</t>
+        </is>
+      </c>
+      <c r="F393" t="inlineStr">
+        <is>
+          <t>https://www.mapacultural.pe.gov.br/files/agent/39532/file/751981/blob-d05bf665f1c96a687e15e77668350fab.png</t>
+        </is>
+      </c>
+      <c r="G393" t="inlineStr">
+        <is>
+          <t>Marcelo Stallone Monteiro Balbino dos Santos</t>
+        </is>
+      </c>
+    </row>
+    <row r="394">
+      <c r="A394" t="inlineStr">
+        <is>
+          <t>Artista Marcelo Stallone</t>
+        </is>
+      </c>
+      <c r="B394" t="inlineStr">
+        <is>
+          <t>CPF</t>
+        </is>
+      </c>
+      <c r="C394" t="inlineStr">
+        <is>
+          <t>Não Feito</t>
+        </is>
+      </c>
+      <c r="D394" t="inlineStr">
+        <is>
+          <t>01/09/2023 às 17:57</t>
+        </is>
+      </c>
+      <c r="E394" t="inlineStr">
+        <is>
+          <t>https://www.mapacultural.pe.gov.br/agente/39532/</t>
+        </is>
+      </c>
+      <c r="F394" t="inlineStr">
+        <is>
+          <t>https://www.mapacultural.pe.gov.br/files/agent/39532/file/751981/blob-d05bf665f1c96a687e15e77668350fab.png</t>
+        </is>
+      </c>
+      <c r="G394" t="inlineStr">
+        <is>
+          <t>Marcelo Stallone Monteiro Balbino dos Santos</t>
+        </is>
+      </c>
+    </row>
+    <row r="395">
+      <c r="A395" t="inlineStr">
+        <is>
+          <t>Artista Marcelo Stallone</t>
+        </is>
+      </c>
+      <c r="B395" t="inlineStr">
+        <is>
+          <t>Comprovante de Residência Atual</t>
+        </is>
+      </c>
+      <c r="C395" t="inlineStr">
+        <is>
+          <t>Não Feito</t>
+        </is>
+      </c>
+      <c r="D395" t="inlineStr">
+        <is>
+          <t>01/09/2023 às 17:57</t>
+        </is>
+      </c>
+      <c r="E395" t="inlineStr">
+        <is>
+          <t>https://www.mapacultural.pe.gov.br/agente/39532/</t>
+        </is>
+      </c>
+      <c r="F395" t="inlineStr">
+        <is>
+          <t>https://www.mapacultural.pe.gov.br/files/agent/39532/file/751981/blob-d05bf665f1c96a687e15e77668350fab.png</t>
+        </is>
+      </c>
+      <c r="G395" t="inlineStr">
+        <is>
+          <t>Marcelo Stallone Monteiro Balbino dos Santos</t>
+        </is>
+      </c>
+    </row>
+    <row r="396">
+      <c r="A396" t="inlineStr">
+        <is>
+          <t>Artista Marcelo Stallone</t>
+        </is>
+      </c>
+      <c r="B396" t="inlineStr">
+        <is>
+          <t>Comprovações Artísticas</t>
+        </is>
+      </c>
+      <c r="C396" t="inlineStr">
+        <is>
+          <t>Não Feito</t>
+        </is>
+      </c>
+      <c r="D396" t="inlineStr">
+        <is>
+          <t>01/09/2023 às 17:57</t>
+        </is>
+      </c>
+      <c r="E396" t="inlineStr">
+        <is>
+          <t>https://www.mapacultural.pe.gov.br/agente/39532/</t>
+        </is>
+      </c>
+      <c r="F396" t="inlineStr">
+        <is>
+          <t>https://www.mapacultural.pe.gov.br/files/agent/39532/file/751981/blob-d05bf665f1c96a687e15e77668350fab.png</t>
+        </is>
+      </c>
+      <c r="G396" t="inlineStr">
+        <is>
+          <t>Marcelo Stallone Monteiro Balbino dos Santos</t>
+        </is>
+      </c>
+    </row>
+    <row r="397">
+      <c r="A397" t="inlineStr">
+        <is>
+          <t>Artista Marcelo Stallone</t>
+        </is>
+      </c>
+      <c r="B397" t="inlineStr">
+        <is>
+          <t>Currículo Artístico</t>
+        </is>
+      </c>
+      <c r="C397" t="inlineStr">
+        <is>
+          <t>Não Feito</t>
+        </is>
+      </c>
+      <c r="D397" t="inlineStr">
+        <is>
+          <t>01/09/2023 às 17:57</t>
+        </is>
+      </c>
+      <c r="E397" t="inlineStr">
+        <is>
+          <t>https://www.mapacultural.pe.gov.br/agente/39532/</t>
+        </is>
+      </c>
+      <c r="F397" t="inlineStr">
+        <is>
+          <t>https://www.mapacultural.pe.gov.br/files/agent/39532/file/751981/blob-d05bf665f1c96a687e15e77668350fab.png</t>
+        </is>
+      </c>
+      <c r="G397" t="inlineStr">
+        <is>
+          <t>Marcelo Stallone Monteiro Balbino dos Santos</t>
+        </is>
+      </c>
+    </row>
+    <row r="398">
+      <c r="A398" t="inlineStr">
+        <is>
+          <t>Artista Marcelo Stallone</t>
+        </is>
+      </c>
+      <c r="B398" t="inlineStr">
+        <is>
+          <t>Histórico Atualizado (Ano de Início)</t>
+        </is>
+      </c>
+      <c r="C398" t="inlineStr">
+        <is>
+          <t>Não Feito</t>
+        </is>
+      </c>
+      <c r="D398" t="inlineStr">
+        <is>
+          <t>01/09/2023 às 17:57</t>
+        </is>
+      </c>
+      <c r="E398" t="inlineStr">
+        <is>
+          <t>https://www.mapacultural.pe.gov.br/agente/39532/</t>
+        </is>
+      </c>
+      <c r="F398" t="inlineStr">
+        <is>
+          <t>https://www.mapacultural.pe.gov.br/files/agent/39532/file/751981/blob-d05bf665f1c96a687e15e77668350fab.png</t>
+        </is>
+      </c>
+      <c r="G398" t="inlineStr">
+        <is>
+          <t>Marcelo Stallone Monteiro Balbino dos Santos</t>
+        </is>
+      </c>
+    </row>
+    <row r="399">
+      <c r="A399" t="inlineStr">
+        <is>
+          <t>Artista Marcelo Stallone</t>
+        </is>
+      </c>
+      <c r="B399" t="inlineStr">
+        <is>
+          <t>Cadastro Mapa Cultural</t>
+        </is>
+      </c>
+      <c r="C399" t="inlineStr">
+        <is>
+          <t>Feito</t>
+        </is>
+      </c>
+      <c r="D399" t="inlineStr">
+        <is>
+          <t>01/09/2023 às 17:57</t>
+        </is>
+      </c>
+      <c r="E399" t="inlineStr">
+        <is>
+          <t>https://www.mapacultural.pe.gov.br/agente/39532/</t>
+        </is>
+      </c>
+      <c r="F399" t="inlineStr">
+        <is>
+          <t>https://www.mapacultural.pe.gov.br/files/agent/39532/file/751981/blob-d05bf665f1c96a687e15e77668350fab.png</t>
+        </is>
+      </c>
+      <c r="G399" t="inlineStr">
+        <is>
+          <t>Marcelo Stallone Monteiro Balbino dos Santos</t>
+        </is>
+      </c>
+    </row>
+    <row r="400">
+      <c r="A400" t="inlineStr">
+        <is>
+          <t>Artista Marcelo Stallone</t>
+        </is>
+      </c>
+      <c r="B400" t="inlineStr">
+        <is>
+          <t>Número Telefone</t>
+        </is>
+      </c>
+      <c r="C400" t="inlineStr">
+        <is>
+          <t>Não Feito</t>
+        </is>
+      </c>
+      <c r="D400" t="inlineStr">
+        <is>
+          <t>01/09/2023 às 17:57</t>
+        </is>
+      </c>
+      <c r="E400" t="inlineStr">
+        <is>
+          <t>https://www.mapacultural.pe.gov.br/agente/39532/</t>
+        </is>
+      </c>
+      <c r="F400" t="inlineStr">
+        <is>
+          <t>https://www.mapacultural.pe.gov.br/files/agent/39532/file/751981/blob-d05bf665f1c96a687e15e77668350fab.png</t>
+        </is>
+      </c>
+      <c r="G400" t="inlineStr">
+        <is>
+          <t>Marcelo Stallone Monteiro Balbino dos Santos</t>
+        </is>
+      </c>
+    </row>
+    <row r="401">
+      <c r="A401" t="inlineStr">
+        <is>
+          <t>Artista Marcelo Stallone</t>
+        </is>
+      </c>
+      <c r="B401" t="inlineStr">
+        <is>
+          <t>Cor</t>
+        </is>
+      </c>
+      <c r="C401" t="inlineStr">
+        <is>
+          <t>Não Feito</t>
+        </is>
+      </c>
+      <c r="D401" t="inlineStr">
+        <is>
+          <t>01/09/2023 às 17:57</t>
+        </is>
+      </c>
+      <c r="E401" t="inlineStr">
+        <is>
+          <t>https://www.mapacultural.pe.gov.br/agente/39532/</t>
+        </is>
+      </c>
+      <c r="F401" t="inlineStr">
+        <is>
+          <t>https://www.mapacultural.pe.gov.br/files/agent/39532/file/751981/blob-d05bf665f1c96a687e15e77668350fab.png</t>
+        </is>
+      </c>
+      <c r="G401" t="inlineStr">
+        <is>
+          <t>Marcelo Stallone Monteiro Balbino dos Santos</t>
+        </is>
+      </c>
+    </row>
+    <row r="402">
+      <c r="A402" t="inlineStr">
+        <is>
+          <t>Artista Marcelo Stallone</t>
+        </is>
+      </c>
+      <c r="B402" t="inlineStr">
+        <is>
+          <t>Gênero</t>
+        </is>
+      </c>
+      <c r="C402" t="inlineStr">
+        <is>
+          <t>Não Feito</t>
+        </is>
+      </c>
+      <c r="D402" t="inlineStr">
+        <is>
+          <t>01/09/2023 às 17:57</t>
+        </is>
+      </c>
+      <c r="E402" t="inlineStr">
+        <is>
+          <t>https://www.mapacultural.pe.gov.br/agente/39532/</t>
+        </is>
+      </c>
+      <c r="F402" t="inlineStr">
+        <is>
+          <t>https://www.mapacultural.pe.gov.br/files/agent/39532/file/751981/blob-d05bf665f1c96a687e15e77668350fab.png</t>
+        </is>
+      </c>
+      <c r="G402" t="inlineStr">
+        <is>
+          <t>Marcelo Stallone Monteiro Balbino dos Santos</t>
+        </is>
+      </c>
+    </row>
+    <row r="403">
+      <c r="A403" t="inlineStr">
+        <is>
+          <t>Artista Marcelo Stallone</t>
+        </is>
+      </c>
+      <c r="B403" t="inlineStr">
+        <is>
+          <t>Grau de Escolaridade</t>
+        </is>
+      </c>
+      <c r="C403" t="inlineStr">
+        <is>
+          <t>Não Feito</t>
+        </is>
+      </c>
+      <c r="D403" t="inlineStr">
+        <is>
+          <t>01/09/2023 às 17:57</t>
+        </is>
+      </c>
+      <c r="E403" t="inlineStr">
+        <is>
+          <t>https://www.mapacultural.pe.gov.br/agente/39532/</t>
+        </is>
+      </c>
+      <c r="F403" t="inlineStr">
+        <is>
+          <t>https://www.mapacultural.pe.gov.br/files/agent/39532/file/751981/blob-d05bf665f1c96a687e15e77668350fab.png</t>
+        </is>
+      </c>
+      <c r="G403" t="inlineStr">
+        <is>
+          <t>Marcelo Stallone Monteiro Balbino dos Santos</t>
+        </is>
+      </c>
+    </row>
+    <row r="404">
+      <c r="A404" t="inlineStr">
+        <is>
+          <t>Artista Marcelo Stallone</t>
+        </is>
+      </c>
+      <c r="B404" t="inlineStr">
+        <is>
+          <t>Recebe algum benefício do governo?</t>
+        </is>
+      </c>
+      <c r="C404" t="inlineStr">
+        <is>
+          <t>Não Feito</t>
+        </is>
+      </c>
+      <c r="D404" t="inlineStr">
+        <is>
+          <t>01/09/2023 às 17:57</t>
+        </is>
+      </c>
+      <c r="E404" t="inlineStr">
+        <is>
+          <t>https://www.mapacultural.pe.gov.br/agente/39532/</t>
+        </is>
+      </c>
+      <c r="F404" t="inlineStr">
+        <is>
+          <t>https://www.mapacultural.pe.gov.br/files/agent/39532/file/751981/blob-d05bf665f1c96a687e15e77668350fab.png</t>
+        </is>
+      </c>
+      <c r="G404" t="inlineStr">
+        <is>
+          <t>Marcelo Stallone Monteiro Balbino dos Santos</t>
+        </is>
+      </c>
+    </row>
+    <row r="405">
+      <c r="A405" t="inlineStr">
+        <is>
+          <t>Artista Marcelo Stallone</t>
+        </is>
+      </c>
+      <c r="B405" t="inlineStr">
+        <is>
+          <t>Recebeu recursos públicos últimos 5 anos?</t>
+        </is>
+      </c>
+      <c r="C405" t="inlineStr">
+        <is>
+          <t>Não Feito</t>
+        </is>
+      </c>
+      <c r="D405" t="inlineStr">
+        <is>
+          <t>01/09/2023 às 17:57</t>
+        </is>
+      </c>
+      <c r="E405" t="inlineStr">
+        <is>
+          <t>https://www.mapacultural.pe.gov.br/agente/39532/</t>
+        </is>
+      </c>
+      <c r="F405" t="inlineStr">
+        <is>
+          <t>https://www.mapacultural.pe.gov.br/files/agent/39532/file/751981/blob-d05bf665f1c96a687e15e77668350fab.png</t>
+        </is>
+      </c>
+      <c r="G405" t="inlineStr">
+        <is>
+          <t>Marcelo Stallone Monteiro Balbino dos Santos</t>
+        </is>
+      </c>
+    </row>
+    <row r="406">
+      <c r="A406" t="inlineStr">
+        <is>
+          <t>AA TESTE</t>
+        </is>
+      </c>
+      <c r="B406" t="inlineStr">
+        <is>
+          <t>teste 1</t>
+        </is>
+      </c>
+      <c r="C406" t="inlineStr">
+        <is>
+          <t>Não Feito</t>
+        </is>
+      </c>
+      <c r="D406" t="inlineStr">
+        <is>
+          <t>01/09/2023 às 21:36</t>
+        </is>
+      </c>
+      <c r="E406" t="inlineStr"/>
+      <c r="F406" t="inlineStr"/>
+      <c r="G406" t="inlineStr"/>
+    </row>
+    <row r="407">
+      <c r="A407" t="inlineStr">
+        <is>
+          <t>AA TESTE</t>
+        </is>
+      </c>
+      <c r="B407" t="inlineStr">
+        <is>
+          <t>teste 2</t>
+        </is>
+      </c>
+      <c r="C407" t="inlineStr">
+        <is>
+          <t>Feito</t>
+        </is>
+      </c>
+      <c r="D407" t="inlineStr">
+        <is>
+          <t>01/09/2023 às 21:36</t>
+        </is>
+      </c>
+      <c r="E407" t="inlineStr"/>
+      <c r="F407" t="inlineStr"/>
+      <c r="G407" t="inlineStr"/>
+    </row>
+    <row r="408">
+      <c r="A408" t="inlineStr">
+        <is>
+          <t>AA TESTE</t>
+        </is>
+      </c>
+      <c r="B408" t="inlineStr">
+        <is>
+          <t>teste 3</t>
+        </is>
+      </c>
+      <c r="C408" t="inlineStr">
+        <is>
+          <t>Não Feito</t>
+        </is>
+      </c>
+      <c r="D408" t="inlineStr">
+        <is>
+          <t>01/09/2023 às 21:36</t>
+        </is>
+      </c>
+      <c r="E408" t="inlineStr"/>
+      <c r="F408" t="inlineStr"/>
+      <c r="G408" t="inlineStr"/>
+    </row>
+    <row r="409">
+      <c r="A409" t="inlineStr">
+        <is>
+          <t>AA TESTE</t>
+        </is>
+      </c>
+      <c r="B409" t="inlineStr">
+        <is>
+          <t>teste 4</t>
+        </is>
+      </c>
+      <c r="C409" t="inlineStr">
+        <is>
+          <t>Não Feito</t>
+        </is>
+      </c>
+      <c r="D409" t="inlineStr">
+        <is>
+          <t>01/09/2023 às 21:36</t>
+        </is>
+      </c>
+      <c r="E409" t="inlineStr"/>
+      <c r="F409" t="inlineStr"/>
+      <c r="G409" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
minera cidade no mapa e adiciona proponente
</commit_message>
<xml_diff>
--- a/backup_projetos.xlsx
+++ b/backup_projetos.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G409"/>
+  <dimension ref="A1:G405"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -964,7 +964,7 @@
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>Não Feito</t>
+          <t>Feito</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
@@ -972,9 +972,21 @@
           <t>01/09/2023 às 00:57</t>
         </is>
       </c>
-      <c r="E15" t="inlineStr"/>
-      <c r="F15" t="inlineStr"/>
-      <c r="G15" t="inlineStr"/>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>https://www.mapacultural.pe.gov.br/agente/593/</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>https://www.mapacultural.pe.gov.br/files/agent/593/file/1151869/blob.-2-5a26c036add54f2b5171661a842d970e.png</t>
+        </is>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>SHIRLEYDE ALBUQUERQUE</t>
+        </is>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -989,7 +1001,7 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>Não Feito</t>
+          <t>Feito</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
@@ -997,9 +1009,21 @@
           <t>01/09/2023 às 00:57</t>
         </is>
       </c>
-      <c r="E16" t="inlineStr"/>
-      <c r="F16" t="inlineStr"/>
-      <c r="G16" t="inlineStr"/>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>https://www.mapacultural.pe.gov.br/agente/593/</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>https://www.mapacultural.pe.gov.br/files/agent/593/file/1151869/blob.-2-5a26c036add54f2b5171661a842d970e.png</t>
+        </is>
+      </c>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>SHIRLEYDE ALBUQUERQUE</t>
+        </is>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -1014,7 +1038,7 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>Não Feito</t>
+          <t>Feito</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
@@ -1022,9 +1046,21 @@
           <t>01/09/2023 às 00:57</t>
         </is>
       </c>
-      <c r="E17" t="inlineStr"/>
-      <c r="F17" t="inlineStr"/>
-      <c r="G17" t="inlineStr"/>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>https://www.mapacultural.pe.gov.br/agente/593/</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>https://www.mapacultural.pe.gov.br/files/agent/593/file/1151869/blob.-2-5a26c036add54f2b5171661a842d970e.png</t>
+        </is>
+      </c>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>SHIRLEYDE ALBUQUERQUE</t>
+        </is>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -1039,7 +1075,7 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>Não Feito</t>
+          <t>Feito</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
@@ -1047,9 +1083,21 @@
           <t>01/09/2023 às 00:57</t>
         </is>
       </c>
-      <c r="E18" t="inlineStr"/>
-      <c r="F18" t="inlineStr"/>
-      <c r="G18" t="inlineStr"/>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>https://www.mapacultural.pe.gov.br/agente/593/</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>https://www.mapacultural.pe.gov.br/files/agent/593/file/1151869/blob.-2-5a26c036add54f2b5171661a842d970e.png</t>
+        </is>
+      </c>
+      <c r="G18" t="inlineStr">
+        <is>
+          <t>SHIRLEYDE ALBUQUERQUE</t>
+        </is>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
@@ -1064,7 +1112,7 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>Não Feito</t>
+          <t>Feito</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
@@ -1072,9 +1120,21 @@
           <t>01/09/2023 às 00:57</t>
         </is>
       </c>
-      <c r="E19" t="inlineStr"/>
-      <c r="F19" t="inlineStr"/>
-      <c r="G19" t="inlineStr"/>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>https://www.mapacultural.pe.gov.br/agente/593/</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>https://www.mapacultural.pe.gov.br/files/agent/593/file/1151869/blob.-2-5a26c036add54f2b5171661a842d970e.png</t>
+        </is>
+      </c>
+      <c r="G19" t="inlineStr">
+        <is>
+          <t>SHIRLEYDE ALBUQUERQUE</t>
+        </is>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -1089,7 +1149,7 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>Não Feito</t>
+          <t>Feito</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
@@ -1097,9 +1157,21 @@
           <t>01/09/2023 às 00:57</t>
         </is>
       </c>
-      <c r="E20" t="inlineStr"/>
-      <c r="F20" t="inlineStr"/>
-      <c r="G20" t="inlineStr"/>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>https://www.mapacultural.pe.gov.br/agente/593/</t>
+        </is>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>https://www.mapacultural.pe.gov.br/files/agent/593/file/1151869/blob.-2-5a26c036add54f2b5171661a842d970e.png</t>
+        </is>
+      </c>
+      <c r="G20" t="inlineStr">
+        <is>
+          <t>SHIRLEYDE ALBUQUERQUE</t>
+        </is>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -1114,7 +1186,7 @@
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>Não Feito</t>
+          <t>Feito</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
@@ -1122,9 +1194,21 @@
           <t>01/09/2023 às 00:57</t>
         </is>
       </c>
-      <c r="E21" t="inlineStr"/>
-      <c r="F21" t="inlineStr"/>
-      <c r="G21" t="inlineStr"/>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>https://www.mapacultural.pe.gov.br/agente/593/</t>
+        </is>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>https://www.mapacultural.pe.gov.br/files/agent/593/file/1151869/blob.-2-5a26c036add54f2b5171661a842d970e.png</t>
+        </is>
+      </c>
+      <c r="G21" t="inlineStr">
+        <is>
+          <t>SHIRLEYDE ALBUQUERQUE</t>
+        </is>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -1139,7 +1223,7 @@
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>Não Feito</t>
+          <t>Feito</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
@@ -1147,9 +1231,21 @@
           <t>01/09/2023 às 00:57</t>
         </is>
       </c>
-      <c r="E22" t="inlineStr"/>
-      <c r="F22" t="inlineStr"/>
-      <c r="G22" t="inlineStr"/>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>https://www.mapacultural.pe.gov.br/agente/593/</t>
+        </is>
+      </c>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>https://www.mapacultural.pe.gov.br/files/agent/593/file/1151869/blob.-2-5a26c036add54f2b5171661a842d970e.png</t>
+        </is>
+      </c>
+      <c r="G22" t="inlineStr">
+        <is>
+          <t>SHIRLEYDE ALBUQUERQUE</t>
+        </is>
+      </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
@@ -1164,7 +1260,7 @@
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>Não Feito</t>
+          <t>Feito</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
@@ -1172,9 +1268,21 @@
           <t>01/09/2023 às 00:57</t>
         </is>
       </c>
-      <c r="E23" t="inlineStr"/>
-      <c r="F23" t="inlineStr"/>
-      <c r="G23" t="inlineStr"/>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>https://www.mapacultural.pe.gov.br/agente/593/</t>
+        </is>
+      </c>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>https://www.mapacultural.pe.gov.br/files/agent/593/file/1151869/blob.-2-5a26c036add54f2b5171661a842d970e.png</t>
+        </is>
+      </c>
+      <c r="G23" t="inlineStr">
+        <is>
+          <t>SHIRLEYDE ALBUQUERQUE</t>
+        </is>
+      </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
@@ -1189,7 +1297,7 @@
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>Não Feito</t>
+          <t>Feito</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
@@ -1197,9 +1305,21 @@
           <t>01/09/2023 às 00:57</t>
         </is>
       </c>
-      <c r="E24" t="inlineStr"/>
-      <c r="F24" t="inlineStr"/>
-      <c r="G24" t="inlineStr"/>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>https://www.mapacultural.pe.gov.br/agente/593/</t>
+        </is>
+      </c>
+      <c r="F24" t="inlineStr">
+        <is>
+          <t>https://www.mapacultural.pe.gov.br/files/agent/593/file/1151869/blob.-2-5a26c036add54f2b5171661a842d970e.png</t>
+        </is>
+      </c>
+      <c r="G24" t="inlineStr">
+        <is>
+          <t>SHIRLEYDE ALBUQUERQUE</t>
+        </is>
+      </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
@@ -1214,7 +1334,7 @@
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>Não Feito</t>
+          <t>Feito</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
@@ -1222,9 +1342,21 @@
           <t>01/09/2023 às 00:57</t>
         </is>
       </c>
-      <c r="E25" t="inlineStr"/>
-      <c r="F25" t="inlineStr"/>
-      <c r="G25" t="inlineStr"/>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>https://www.mapacultural.pe.gov.br/agente/593/</t>
+        </is>
+      </c>
+      <c r="F25" t="inlineStr">
+        <is>
+          <t>https://www.mapacultural.pe.gov.br/files/agent/593/file/1151869/blob.-2-5a26c036add54f2b5171661a842d970e.png</t>
+        </is>
+      </c>
+      <c r="G25" t="inlineStr">
+        <is>
+          <t>SHIRLEYDE ALBUQUERQUE</t>
+        </is>
+      </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
@@ -1239,7 +1371,7 @@
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>Não Feito</t>
+          <t>Feito</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
@@ -1247,9 +1379,21 @@
           <t>01/09/2023 às 00:57</t>
         </is>
       </c>
-      <c r="E26" t="inlineStr"/>
-      <c r="F26" t="inlineStr"/>
-      <c r="G26" t="inlineStr"/>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>https://www.mapacultural.pe.gov.br/agente/593/</t>
+        </is>
+      </c>
+      <c r="F26" t="inlineStr">
+        <is>
+          <t>https://www.mapacultural.pe.gov.br/files/agent/593/file/1151869/blob.-2-5a26c036add54f2b5171661a842d970e.png</t>
+        </is>
+      </c>
+      <c r="G26" t="inlineStr">
+        <is>
+          <t>SHIRLEYDE ALBUQUERQUE</t>
+        </is>
+      </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
@@ -1264,7 +1408,7 @@
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>Não Feito</t>
+          <t>Feito</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
@@ -1272,9 +1416,21 @@
           <t>01/09/2023 às 00:57</t>
         </is>
       </c>
-      <c r="E27" t="inlineStr"/>
-      <c r="F27" t="inlineStr"/>
-      <c r="G27" t="inlineStr"/>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>https://www.mapacultural.pe.gov.br/agente/593/</t>
+        </is>
+      </c>
+      <c r="F27" t="inlineStr">
+        <is>
+          <t>https://www.mapacultural.pe.gov.br/files/agent/593/file/1151869/blob.-2-5a26c036add54f2b5171661a842d970e.png</t>
+        </is>
+      </c>
+      <c r="G27" t="inlineStr">
+        <is>
+          <t>SHIRLEYDE ALBUQUERQUE</t>
+        </is>
+      </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
@@ -10728,12 +10884,12 @@
       </c>
       <c r="F380" t="inlineStr">
         <is>
-          <t>https://www.mapacultural.pe.gov.br/assets/www.mapacultural.pe.gov.br/img/avatar--agent-2487234669-1693235595.png</t>
+          <t>https://www.mapacultural.pe.gov.br/files/agent/16301/file/1170727/blob.-2-e50ddac85ec7945ec2518f56a4d1b778.png</t>
         </is>
       </c>
       <c r="G380" t="inlineStr">
         <is>
-          <t>elisangela monteiro de melo costa</t>
+          <t>Elisangela Monteiro De Melo Costa</t>
         </is>
       </c>
     </row>
@@ -10765,12 +10921,12 @@
       </c>
       <c r="F381" t="inlineStr">
         <is>
-          <t>https://www.mapacultural.pe.gov.br/assets/www.mapacultural.pe.gov.br/img/avatar--agent-2487234669-1693235595.png</t>
+          <t>https://www.mapacultural.pe.gov.br/files/agent/16301/file/1170727/blob.-2-e50ddac85ec7945ec2518f56a4d1b778.png</t>
         </is>
       </c>
       <c r="G381" t="inlineStr">
         <is>
-          <t>elisangela monteiro de melo costa</t>
+          <t>Elisangela Monteiro De Melo Costa</t>
         </is>
       </c>
     </row>
@@ -10802,12 +10958,12 @@
       </c>
       <c r="F382" t="inlineStr">
         <is>
-          <t>https://www.mapacultural.pe.gov.br/assets/www.mapacultural.pe.gov.br/img/avatar--agent-2487234669-1693235595.png</t>
+          <t>https://www.mapacultural.pe.gov.br/files/agent/16301/file/1170727/blob.-2-e50ddac85ec7945ec2518f56a4d1b778.png</t>
         </is>
       </c>
       <c r="G382" t="inlineStr">
         <is>
-          <t>elisangela monteiro de melo costa</t>
+          <t>Elisangela Monteiro De Melo Costa</t>
         </is>
       </c>
     </row>
@@ -10839,12 +10995,12 @@
       </c>
       <c r="F383" t="inlineStr">
         <is>
-          <t>https://www.mapacultural.pe.gov.br/assets/www.mapacultural.pe.gov.br/img/avatar--agent-2487234669-1693235595.png</t>
+          <t>https://www.mapacultural.pe.gov.br/files/agent/16301/file/1170727/blob.-2-e50ddac85ec7945ec2518f56a4d1b778.png</t>
         </is>
       </c>
       <c r="G383" t="inlineStr">
         <is>
-          <t>elisangela monteiro de melo costa</t>
+          <t>Elisangela Monteiro De Melo Costa</t>
         </is>
       </c>
     </row>
@@ -10876,12 +11032,12 @@
       </c>
       <c r="F384" t="inlineStr">
         <is>
-          <t>https://www.mapacultural.pe.gov.br/assets/www.mapacultural.pe.gov.br/img/avatar--agent-2487234669-1693235595.png</t>
+          <t>https://www.mapacultural.pe.gov.br/files/agent/16301/file/1170727/blob.-2-e50ddac85ec7945ec2518f56a4d1b778.png</t>
         </is>
       </c>
       <c r="G384" t="inlineStr">
         <is>
-          <t>elisangela monteiro de melo costa</t>
+          <t>Elisangela Monteiro De Melo Costa</t>
         </is>
       </c>
     </row>
@@ -10913,12 +11069,12 @@
       </c>
       <c r="F385" t="inlineStr">
         <is>
-          <t>https://www.mapacultural.pe.gov.br/assets/www.mapacultural.pe.gov.br/img/avatar--agent-2487234669-1693235595.png</t>
+          <t>https://www.mapacultural.pe.gov.br/files/agent/16301/file/1170727/blob.-2-e50ddac85ec7945ec2518f56a4d1b778.png</t>
         </is>
       </c>
       <c r="G385" t="inlineStr">
         <is>
-          <t>elisangela monteiro de melo costa</t>
+          <t>Elisangela Monteiro De Melo Costa</t>
         </is>
       </c>
     </row>
@@ -10950,12 +11106,12 @@
       </c>
       <c r="F386" t="inlineStr">
         <is>
-          <t>https://www.mapacultural.pe.gov.br/assets/www.mapacultural.pe.gov.br/img/avatar--agent-2487234669-1693235595.png</t>
+          <t>https://www.mapacultural.pe.gov.br/files/agent/16301/file/1170727/blob.-2-e50ddac85ec7945ec2518f56a4d1b778.png</t>
         </is>
       </c>
       <c r="G386" t="inlineStr">
         <is>
-          <t>elisangela monteiro de melo costa</t>
+          <t>Elisangela Monteiro De Melo Costa</t>
         </is>
       </c>
     </row>
@@ -10987,12 +11143,12 @@
       </c>
       <c r="F387" t="inlineStr">
         <is>
-          <t>https://www.mapacultural.pe.gov.br/assets/www.mapacultural.pe.gov.br/img/avatar--agent-2487234669-1693235595.png</t>
+          <t>https://www.mapacultural.pe.gov.br/files/agent/16301/file/1170727/blob.-2-e50ddac85ec7945ec2518f56a4d1b778.png</t>
         </is>
       </c>
       <c r="G387" t="inlineStr">
         <is>
-          <t>elisangela monteiro de melo costa</t>
+          <t>Elisangela Monteiro De Melo Costa</t>
         </is>
       </c>
     </row>
@@ -11024,12 +11180,12 @@
       </c>
       <c r="F388" t="inlineStr">
         <is>
-          <t>https://www.mapacultural.pe.gov.br/assets/www.mapacultural.pe.gov.br/img/avatar--agent-2487234669-1693235595.png</t>
+          <t>https://www.mapacultural.pe.gov.br/files/agent/16301/file/1170727/blob.-2-e50ddac85ec7945ec2518f56a4d1b778.png</t>
         </is>
       </c>
       <c r="G388" t="inlineStr">
         <is>
-          <t>elisangela monteiro de melo costa</t>
+          <t>Elisangela Monteiro De Melo Costa</t>
         </is>
       </c>
     </row>
@@ -11061,12 +11217,12 @@
       </c>
       <c r="F389" t="inlineStr">
         <is>
-          <t>https://www.mapacultural.pe.gov.br/assets/www.mapacultural.pe.gov.br/img/avatar--agent-2487234669-1693235595.png</t>
+          <t>https://www.mapacultural.pe.gov.br/files/agent/16301/file/1170727/blob.-2-e50ddac85ec7945ec2518f56a4d1b778.png</t>
         </is>
       </c>
       <c r="G389" t="inlineStr">
         <is>
-          <t>elisangela monteiro de melo costa</t>
+          <t>Elisangela Monteiro De Melo Costa</t>
         </is>
       </c>
     </row>
@@ -11098,12 +11254,12 @@
       </c>
       <c r="F390" t="inlineStr">
         <is>
-          <t>https://www.mapacultural.pe.gov.br/assets/www.mapacultural.pe.gov.br/img/avatar--agent-2487234669-1693235595.png</t>
+          <t>https://www.mapacultural.pe.gov.br/files/agent/16301/file/1170727/blob.-2-e50ddac85ec7945ec2518f56a4d1b778.png</t>
         </is>
       </c>
       <c r="G390" t="inlineStr">
         <is>
-          <t>elisangela monteiro de melo costa</t>
+          <t>Elisangela Monteiro De Melo Costa</t>
         </is>
       </c>
     </row>
@@ -11135,12 +11291,12 @@
       </c>
       <c r="F391" t="inlineStr">
         <is>
-          <t>https://www.mapacultural.pe.gov.br/assets/www.mapacultural.pe.gov.br/img/avatar--agent-2487234669-1693235595.png</t>
+          <t>https://www.mapacultural.pe.gov.br/files/agent/16301/file/1170727/blob.-2-e50ddac85ec7945ec2518f56a4d1b778.png</t>
         </is>
       </c>
       <c r="G391" t="inlineStr">
         <is>
-          <t>elisangela monteiro de melo costa</t>
+          <t>Elisangela Monteiro De Melo Costa</t>
         </is>
       </c>
     </row>
@@ -11172,12 +11328,12 @@
       </c>
       <c r="F392" t="inlineStr">
         <is>
-          <t>https://www.mapacultural.pe.gov.br/assets/www.mapacultural.pe.gov.br/img/avatar--agent-2487234669-1693235595.png</t>
+          <t>https://www.mapacultural.pe.gov.br/files/agent/16301/file/1170727/blob.-2-e50ddac85ec7945ec2518f56a4d1b778.png</t>
         </is>
       </c>
       <c r="G392" t="inlineStr">
         <is>
-          <t>elisangela monteiro de melo costa</t>
+          <t>Elisangela Monteiro De Melo Costa</t>
         </is>
       </c>
     </row>
@@ -11661,106 +11817,6 @@
           <t>Marcelo Stallone Monteiro Balbino dos Santos</t>
         </is>
       </c>
-    </row>
-    <row r="406">
-      <c r="A406" t="inlineStr">
-        <is>
-          <t>AA TESTE</t>
-        </is>
-      </c>
-      <c r="B406" t="inlineStr">
-        <is>
-          <t>teste 1</t>
-        </is>
-      </c>
-      <c r="C406" t="inlineStr">
-        <is>
-          <t>Não Feito</t>
-        </is>
-      </c>
-      <c r="D406" t="inlineStr">
-        <is>
-          <t>01/09/2023 às 21:36</t>
-        </is>
-      </c>
-      <c r="E406" t="inlineStr"/>
-      <c r="F406" t="inlineStr"/>
-      <c r="G406" t="inlineStr"/>
-    </row>
-    <row r="407">
-      <c r="A407" t="inlineStr">
-        <is>
-          <t>AA TESTE</t>
-        </is>
-      </c>
-      <c r="B407" t="inlineStr">
-        <is>
-          <t>teste 2</t>
-        </is>
-      </c>
-      <c r="C407" t="inlineStr">
-        <is>
-          <t>Feito</t>
-        </is>
-      </c>
-      <c r="D407" t="inlineStr">
-        <is>
-          <t>01/09/2023 às 21:36</t>
-        </is>
-      </c>
-      <c r="E407" t="inlineStr"/>
-      <c r="F407" t="inlineStr"/>
-      <c r="G407" t="inlineStr"/>
-    </row>
-    <row r="408">
-      <c r="A408" t="inlineStr">
-        <is>
-          <t>AA TESTE</t>
-        </is>
-      </c>
-      <c r="B408" t="inlineStr">
-        <is>
-          <t>teste 3</t>
-        </is>
-      </c>
-      <c r="C408" t="inlineStr">
-        <is>
-          <t>Não Feito</t>
-        </is>
-      </c>
-      <c r="D408" t="inlineStr">
-        <is>
-          <t>01/09/2023 às 21:36</t>
-        </is>
-      </c>
-      <c r="E408" t="inlineStr"/>
-      <c r="F408" t="inlineStr"/>
-      <c r="G408" t="inlineStr"/>
-    </row>
-    <row r="409">
-      <c r="A409" t="inlineStr">
-        <is>
-          <t>AA TESTE</t>
-        </is>
-      </c>
-      <c r="B409" t="inlineStr">
-        <is>
-          <t>teste 4</t>
-        </is>
-      </c>
-      <c r="C409" t="inlineStr">
-        <is>
-          <t>Não Feito</t>
-        </is>
-      </c>
-      <c r="D409" t="inlineStr">
-        <is>
-          <t>01/09/2023 às 21:36</t>
-        </is>
-      </c>
-      <c r="E409" t="inlineStr"/>
-      <c r="F409" t="inlineStr"/>
-      <c r="G409" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>